<commit_message>
SAPP2-163 - Phase 2 Security: Import cart using Bulk order import functionality (NTH) - Template xlsx update
</commit_message>
<xml_diff>
--- a/core-customize/hybris/bin/custom/gallagherb2b/gallagherb2binitialdata/resources/gallagherb2binitialdata/import/coredata/contentCatalogs/securityB2BContentCatalog/documents/BulkOrderTemplate.xlsx
+++ b/core-customize/hybris/bin/custom/gallagherb2b/gallagherb2binitialdata/resources/gallagherb2binitialdata/import/coredata/contentCatalogs/securityB2BContentCatalog/documents/BulkOrderTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ishaanvashishth\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\EWGallagher\core-customize\hybris\bin\custom\gallagherb2b\gallagherb2binitialdata\resources\gallagherb2binitialdata\import\coredata\contentCatalogs\securityB2BContentCatalog\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36267513-B8D4-4AED-9852-90A082010941}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCA4113-0CE1-41E1-8648-CB25A4BCCE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>ProductSKU</t>
+    <t>ProductID</t>
   </si>
 </sst>
 </file>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD26"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>